<commit_message>
completed all of the majors, dates, and races for each file
</commit_message>
<xml_diff>
--- a/VisitDays/major_decoder.xlsx
+++ b/VisitDays/major_decoder.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AsareTheGreat 1/Development/Salesforce/YouVisit Script/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AsareTheGreat 1/Development/DevSalesforce/VisitDays/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F525B3DA-39C4-4E48-98CD-68A6B22F1F3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF2A5FDE-D0A2-F14E-A4AC-7446EF0CB0C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18960" xr2:uid="{BB11F144-B0A3-4BB1-826B-A04BBFEC811F}"/>
   </bookViews>
@@ -5666,9 +5666,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34E247E-339C-4235-A8D6-3D396899836D}">
   <dimension ref="A1:B2311"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5677,7 +5675,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>1702</v>
       </c>
       <c r="B1" s="1" t="s">

</xml_diff>